<commit_message>
Added support for Hi Lo odds.
</commit_message>
<xml_diff>
--- a/oddsbook.xlsx
+++ b/oddsbook.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewis/Workspace/solo/oddsbook-git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E7AB07-FA22-B24C-A136-63DDB197CFE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC3136D-B03C-FB47-A0AF-6F768F3F3F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="24800" windowHeight="15540" xr2:uid="{92800E38-51DD-1645-9321-12A124E08DB0}"/>
+    <workbookView xWindow="16340" yWindow="10760" windowWidth="24800" windowHeight="15540" xr2:uid="{92800E38-51DD-1645-9321-12A124E08DB0}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="全場主客和">TEMPLATE!$A$1</definedName>
+    <definedName name="全場入球大細">TEMPLATE!$K$1</definedName>
     <definedName name="全場讓球">TEMPLATE!$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>主</t>
   </si>
@@ -50,6 +51,18 @@
   </si>
   <si>
     <t>更新時間</t>
+  </si>
+  <si>
+    <t>全場入球大細</t>
+  </si>
+  <si>
+    <t>球數</t>
+  </si>
+  <si>
+    <t>大</t>
+  </si>
+  <si>
+    <t>細</t>
   </si>
 </sst>
 </file>
@@ -405,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10D9BF1-E001-3345-B7D4-DE95DAA3F73D}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -417,15 +430,18 @@
     <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -449,6 +465,18 @@
       </c>
       <c r="I2" t="s">
         <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for Corner Hi Lo odds.
</commit_message>
<xml_diff>
--- a/oddsbook.xlsx
+++ b/oddsbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewis/Workspace/solo/oddsbook-git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC3136D-B03C-FB47-A0AF-6F768F3F3F37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C36E44-D536-944E-B93E-836C929578F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16340" yWindow="10760" windowWidth="24800" windowHeight="15540" xr2:uid="{92800E38-51DD-1645-9321-12A124E08DB0}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   <definedNames>
     <definedName name="全場主客和">TEMPLATE!$A$1</definedName>
     <definedName name="全場入球大細">TEMPLATE!$K$1</definedName>
+    <definedName name="全場角球入球大細">TEMPLATE!$P$1</definedName>
     <definedName name="全場讓球">TEMPLATE!$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>主</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t>細</t>
+  </si>
+  <si>
+    <t>全場角球入球大細</t>
   </si>
 </sst>
 </file>
@@ -418,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B10D9BF1-E001-3345-B7D4-DE95DAA3F73D}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,7 +434,7 @@
     <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -440,8 +444,11 @@
       <c r="K1" t="s">
         <v>7</v>
       </c>
+      <c r="P1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -476,6 +483,18 @@
         <v>9</v>
       </c>
       <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug fix for Corner Hi Lo.
</commit_message>
<xml_diff>
--- a/oddsbook.xlsx
+++ b/oddsbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lewis/Workspace/solo/oddsbook-git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C36E44-D536-944E-B93E-836C929578F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ABA1F8-51B3-0C40-81F3-8C63E7213B94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16340" yWindow="10760" windowWidth="24800" windowHeight="15540" xr2:uid="{92800E38-51DD-1645-9321-12A124E08DB0}"/>
+    <workbookView xWindow="820" yWindow="460" windowWidth="24780" windowHeight="15540" xr2:uid="{92800E38-51DD-1645-9321-12A124E08DB0}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="全場主客和">TEMPLATE!$A$1</definedName>
     <definedName name="全場入球大細">TEMPLATE!$K$1</definedName>
-    <definedName name="全場角球入球大細">TEMPLATE!$P$1</definedName>
+    <definedName name="全場角球大細">TEMPLATE!$P$1</definedName>
     <definedName name="全場讓球">TEMPLATE!$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -66,7 +66,7 @@
     <t>細</t>
   </si>
   <si>
-    <t>全場角球入球大細</t>
+    <t>全場角球大細</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>